<commit_message>
distance sensor still not working perfectly :-(
</commit_message>
<xml_diff>
--- a/Sensor Modules/Distance Sensor/MetricConversion.xlsx
+++ b/Sensor Modules/Distance Sensor/MetricConversion.xlsx
@@ -1,18 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26018"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26207"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Majeed/Dropbox/Professional/Projects/ProjectMakerShoe/Design/MakerWear/2nd Architecture/Modules/Distance Sensor/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Majeed/Dropbox/Professional/Projects/ProjectMakerShoe/Design/MakerWear/2nd Architecture/MakerWear/Sensor Modules/Distance Sensor/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14240" tabRatio="500"/>
+    <workbookView xWindow="12800" yWindow="460" windowWidth="12800" windowHeight="14240" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -21,6 +22,14 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>Nothing</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -405,11 +414,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2133271920"/>
-        <c:axId val="-2136522640"/>
+        <c:axId val="2142882880"/>
+        <c:axId val="2142886272"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2133271920"/>
+        <c:axId val="2142882880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -466,12 +475,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2136522640"/>
+        <c:crossAx val="2142886272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2136522640"/>
+        <c:axId val="2142886272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -528,7 +537,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2133271920"/>
+        <c:crossAx val="2142882880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1433,8 +1442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection sqref="A1:B24"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1636,4 +1645,38 @@
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>950</v>
+      </c>
+      <c r="C1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>975</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>